<commit_message>
Updated BioVal and new RedCap variabled. As well the Lab ID is inculded now.
</commit_message>
<xml_diff>
--- a/templates/Redcap_Biorepos.xlsx
+++ b/templates/Redcap_Biorepos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="93">
   <si>
     <t xml:space="preserve">tube variables</t>
   </si>
@@ -29,184 +29,190 @@
     <t xml:space="preserve">sample variables</t>
   </si>
   <si>
+    <t xml:space="preserve">stud_id</t>
+  </si>
+  <si>
     <t xml:space="preserve">pat_id</t>
   </si>
   <si>
+    <t xml:space="preserve">study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">study_visit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">material</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tube_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">box_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freezer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rack</t>
+  </si>
+  <si>
+    <t xml:space="preserve">box</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fibro_passage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mycoplasma Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HIV / HBV / HCV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">einfrierdatum_minus80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aufgetaut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">volumen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kommentar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verschickt_am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verschickt_empfaenger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verschickt_projekt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reserviert_am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reserviert_fuer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extern_prozessiert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visit_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freeze_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nuechtern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">probenabnahme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aufarbeitung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pat_nr_study</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treatHSP ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interne HD ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treatHSP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1-H12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Freitext</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P1-P4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">negativ / positiv / untested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xx.xx.xxxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja / nein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xx:xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ja / nein / unbekannt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">treatPOLR3A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FU1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSF Pellet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BDNF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FU2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DNA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sonstige</t>
+  </si>
+  <si>
+    <t xml:space="preserve">…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDTA Plasma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nitrogen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fibroblasten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PAXgene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PBMC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Serum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Urin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pflichtfeld</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nicht Pflichfeld</t>
+  </si>
+  <si>
     <t xml:space="preserve">visit_date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">study_visit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">material</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tube_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">box_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">freezer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rack</t>
-  </si>
-  <si>
-    <t xml:space="preserve">box</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fibro_passage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mycoplasma Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIV / HBV / HCV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">einfrierdatum_minus80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aufgetaut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">volumen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kommentar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verschickt_am</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verschickt_empfaenger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verschickt_projekt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reserviert_am</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reserviert_fuer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">extern_prozessiert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">visit_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">freeze_time</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nuechtern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">probenabnahme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aufarbeitung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pat_nr_study</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interne HD ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xx.xx.xxxx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treatHSP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A1-H12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Freitext</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1-100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P1-P4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">negativ / positiv / untested</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja / nein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">xx:xx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ja / nein / unbekannt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">treatPOLR3A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FU1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSF Pellet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BDNF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FU2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DNA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sonstige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">…</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EDTA Plasma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nitrogen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fibroblasten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PAXgene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PBMC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pflichtfeld</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nicht Pflichfeld</t>
   </si>
   <si>
     <t xml:space="preserve">zellzahl_ampulle</t>
@@ -304,7 +310,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="h:mm"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -326,6 +332,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -416,7 +430,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -433,15 +447,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -449,11 +467,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -537,19 +555,18 @@
   <dimension ref="A1:AD17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -581,103 +598,103 @@
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="K2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Y2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AC2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AD2" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -717,10 +734,10 @@
         <v>41</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="0" t="s">
         <v>38</v>
@@ -744,16 +761,16 @@
         <v>38</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Z3" s="7" t="s">
-        <v>43</v>
+      <c r="Y3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z3" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB3" s="0" t="s">
         <v>38</v>
@@ -765,86 +782,86 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C6" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="0" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="0" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="0" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="0" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="4" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="B1:X1"/>
     <mergeCell ref="Y1:AD1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -868,7 +885,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="16.67"/>
@@ -935,181 +952,181 @@
       <c r="BB1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="M2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="N2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="4" t="s">
+      <c r="Q2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="R2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="S2" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="T2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="U2" s="4" t="s">
+      <c r="U2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="V2" s="4" t="s">
+      <c r="V2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="W2" s="4" t="s">
+      <c r="W2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="X2" s="4" t="s">
+      <c r="X2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Y2" s="4" t="s">
+      <c r="Y2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AB2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AC2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AC2" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AE2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AF2" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AF2" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="AH2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="AI2" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AK2" s="9" t="s">
+      <c r="AI2" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="AL2" s="9" t="s">
+      <c r="AJ2" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="AM2" s="9" t="s">
+      <c r="AK2" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="AN2" s="9" t="s">
+      <c r="AL2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="AO2" s="9" t="s">
+      <c r="AM2" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="AP2" s="9" t="s">
+      <c r="AN2" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="AQ2" s="9" t="s">
+      <c r="AO2" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="AR2" s="9" t="s">
+      <c r="AP2" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="AS2" s="9" t="s">
+      <c r="AQ2" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="AT2" s="9" t="s">
+      <c r="AR2" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="AU2" s="9" t="s">
+      <c r="AS2" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="AV2" s="9" t="s">
+      <c r="AT2" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="AW2" s="9" t="s">
+      <c r="AU2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="AX2" s="9" t="s">
+      <c r="AV2" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="AY2" s="9" t="s">
+      <c r="AW2" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="AZ2" s="9" t="s">
+      <c r="AX2" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="BA2" s="9" t="s">
+      <c r="AY2" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="BB2" s="9" t="s">
+      <c r="AZ2" s="10" t="s">
         <v>85</v>
       </c>
+      <c r="BA2" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="BB2" s="10" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>33</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>34</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E3" s="0" t="s">
         <v>36</v>
@@ -1142,10 +1159,10 @@
         <v>41</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="Q3" s="0" t="s">
         <v>38</v>
@@ -1169,16 +1186,16 @@
         <v>38</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="Z3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="AA3" s="7" t="s">
-        <v>43</v>
+      <c r="Z3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>44</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD3" s="0" t="s">
         <v>38</v>
@@ -1192,13 +1209,13 @@
     </row>
     <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I4" s="0" t="n">
         <v>2</v>
@@ -1206,13 +1223,13 @@
     </row>
     <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I5" s="0" t="n">
         <v>3</v>
@@ -1220,38 +1237,38 @@
     </row>
     <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E7" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E11" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>